<commit_message>
Update Pattern assign tests
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test11_Sequential/QuerySet.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test11_Sequential/QuerySet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="68">
   <si>
     <t>Index</t>
   </si>
@@ -102,15 +102,6 @@
     <t>Select BOOLEAN pattern a(_, _"e+d"_)</t>
   </si>
   <si>
-    <t>Select BOOLEAN pattern a(_, _"3*4"_)</t>
-  </si>
-  <si>
-    <t>Select BOOLEAN pattern a(_, _"(c*d)"_)</t>
-  </si>
-  <si>
-    <t>Select BOOLEAN pattern a(_, _"(g+3*4)"_)</t>
-  </si>
-  <si>
     <t>Select BOOLEAN pattern a(_, _"(3*4-6)"_)</t>
   </si>
   <si>
@@ -129,9 +120,6 @@
     <t>Select BOOLEAN pattern a(_, _"((c*a)"_)</t>
   </si>
   <si>
-    <t>Select BOOLEAN pattern a("f", _"e*f"_)</t>
-  </si>
-  <si>
     <t>Ident PartialMatch Expr</t>
   </si>
   <si>
@@ -180,30 +168,12 @@
     <t>Variable PartialMatch</t>
   </si>
   <si>
-    <t>Select v such that pattern a(v, _"b"_)</t>
-  </si>
-  <si>
-    <t>Select v such that pattern a(v, _)</t>
-  </si>
-  <si>
-    <t>Select v such that pattern a(v, "2")</t>
-  </si>
-  <si>
     <t>h</t>
   </si>
   <si>
     <t>Variable ExactMatch</t>
   </si>
   <si>
-    <t>Select a such that pattern a(v, _)</t>
-  </si>
-  <si>
-    <t>Select a such that pattern a(v, _"b"_)</t>
-  </si>
-  <si>
-    <t>Select a such that pattern a(v, "2")</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
@@ -214,6 +184,45 @@
   </si>
   <si>
     <t>2,7,8,11,12,17,23</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN pattern a(_, _"(a+b)"_)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN pattern a(_, _"(f+3)"_)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN pattern a(_, _"2+20*a"_)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN pattern a(_, _"()"_)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN pattern a(_, _"+4"_)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN pattern a(_, _"1-"_)</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN pattern a("f", _"c * b + 2- 5"_)</t>
+  </si>
+  <si>
+    <t>Select v pattern a(v, _)</t>
+  </si>
+  <si>
+    <t>Select v pattern a(v, _"b"_)</t>
+  </si>
+  <si>
+    <t>Select v pattern a(v, "2")</t>
+  </si>
+  <si>
+    <t>Select a pattern a(v, _)</t>
+  </si>
+  <si>
+    <t>Select a pattern a(v, _"b"_)</t>
+  </si>
+  <si>
+    <t>Select a pattern a(v, "2")</t>
   </si>
 </sst>
 </file>
@@ -643,12 +652,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3B02F3-8668-4835-B18A-9EFEA275CE21}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A27"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,16 +700,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F2" s="6"/>
     </row>
@@ -709,16 +718,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F3" s="6"/>
     </row>
@@ -727,16 +736,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F4" s="6"/>
     </row>
@@ -745,7 +754,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>9</v>
@@ -762,7 +771,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>11</v>
@@ -779,7 +788,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>12</v>
@@ -796,7 +805,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>20</v>
@@ -813,7 +822,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>22</v>
@@ -830,7 +839,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>25</v>
@@ -839,7 +848,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F10" s="6"/>
     </row>
@@ -848,7 +857,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>26</v>
@@ -857,7 +866,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F11" s="6"/>
     </row>
@@ -866,16 +875,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F12" s="6"/>
     </row>
@@ -884,16 +893,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F13" s="6"/>
     </row>
@@ -902,16 +911,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F14" s="6"/>
     </row>
@@ -920,16 +929,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F15" s="6"/>
     </row>
@@ -938,195 +947,249 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>61</v>
+        <v>49</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Test 11 final
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test11_Sequential/QuerySet.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test11_Sequential/QuerySet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="313">
   <si>
     <t>Index</t>
   </si>
@@ -567,6 +567,399 @@
   </si>
   <si>
     <t>1,2,3,4,5,6,7,8,9,10,11,13,16,18,22,24</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with 1 = 1</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with 1 = 2</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with 1 = "badstring"</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with 1 = s.stmt#</t>
+  </si>
+  <si>
+    <t>Int Stmt Attr</t>
+  </si>
+  <si>
+    <t>Select BOOLAEN with 2 = a.stmt#</t>
+  </si>
+  <si>
+    <t>Int Assign Attr</t>
+  </si>
+  <si>
+    <t>procedure p;</t>
+  </si>
+  <si>
+    <t>variable v;</t>
+  </si>
+  <si>
+    <t>constant c;</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with 14 = w.stmt#</t>
+  </si>
+  <si>
+    <t>Int While Attr</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with 19 = if.stmt#</t>
+  </si>
+  <si>
+    <t>Int If Attr</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with 18 = pl</t>
+  </si>
+  <si>
+    <t>Int ProgLine Attr</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with 1000 = pl</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with 25 = cl.stmt#</t>
+  </si>
+  <si>
+    <t>Int Call Attr String</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with 12 = cl.procName</t>
+  </si>
+  <si>
+    <t>Int Call Attr Int</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with 4 = p.procName</t>
+  </si>
+  <si>
+    <t>Int Procedure Attr</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with 5 = s.procName</t>
+  </si>
+  <si>
+    <t>Wrong AttrRef</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with 3 = v.varName</t>
+  </si>
+  <si>
+    <t>Int Variable Attr</t>
+  </si>
+  <si>
+    <t>Int Constant Attr</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with 2 = c.value</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with 26 = c.value</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with "badstring" = 1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Constant Int</t>
+  </si>
+  <si>
+    <t>Select s with s.stmt# = 2</t>
+  </si>
+  <si>
+    <t>Select a with a.stmt# = 3</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN with 14 = a.stmt#</t>
+  </si>
+  <si>
+    <t>Select w with w.stmt#=14</t>
+  </si>
+  <si>
+    <t>Select if with if.stmt = 19</t>
+  </si>
+  <si>
+    <t>Select pl with pl = 5</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>ProgLine int</t>
+  </si>
+  <si>
+    <t>Select cl with cl.stmt# = 25</t>
+  </si>
+  <si>
+    <t>Select c with c.value = 3</t>
+  </si>
+  <si>
+    <t>Select s with s.stmt# = a.stmt#</t>
+  </si>
+  <si>
+    <t>Select s with s.stmt# = w.stmt#</t>
+  </si>
+  <si>
+    <t>Select s with s.stmt# = s.stmt#</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26</t>
+  </si>
+  <si>
+    <t>Select s with s.stmt# = f.stmt#</t>
+  </si>
+  <si>
+    <t>stmt s; prog_line pl;</t>
+  </si>
+  <si>
+    <t>Select s with s.stmt# = pl</t>
+  </si>
+  <si>
+    <t>Select s with s.stmt# = cl.stmt#</t>
+  </si>
+  <si>
+    <t>stmt s; constant c;</t>
+  </si>
+  <si>
+    <t>Select s with s.stmt# = c.value</t>
+  </si>
+  <si>
+    <t>Stmt Constant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assign a; </t>
+  </si>
+  <si>
+    <t>Select a with a.stmt# = a.stmt#</t>
+  </si>
+  <si>
+    <t>assign a; if f;</t>
+  </si>
+  <si>
+    <t>Select a with a.stmt# = f.stmt#</t>
+  </si>
+  <si>
+    <t>Select a with a.stmt# = w.stmt#</t>
+  </si>
+  <si>
+    <t>assign a; prog_line pl;</t>
+  </si>
+  <si>
+    <t>Select a with a.stmt# = pl</t>
+  </si>
+  <si>
+    <t>Select a with a.stmt# = cl.stmt#</t>
+  </si>
+  <si>
+    <t>assign a; constant c;</t>
+  </si>
+  <si>
+    <t>Assign Constant</t>
+  </si>
+  <si>
+    <t>Select w with w.stmt#=w.stmt#</t>
+  </si>
+  <si>
+    <t>While While</t>
+  </si>
+  <si>
+    <t>while w; if f;</t>
+  </si>
+  <si>
+    <t>Select w with w.stmt# = f.stmt#</t>
+  </si>
+  <si>
+    <t>While If</t>
+  </si>
+  <si>
+    <t>while w; prog_line pl;</t>
+  </si>
+  <si>
+    <t>Select w with w.stmt# = pl</t>
+  </si>
+  <si>
+    <t>While ProgLine</t>
+  </si>
+  <si>
+    <t>while w; call cl;</t>
+  </si>
+  <si>
+    <t>Select w with w.stmt# = cl.stmt#</t>
+  </si>
+  <si>
+    <t>While Call</t>
+  </si>
+  <si>
+    <t>while w; constant c;</t>
+  </si>
+  <si>
+    <t>Select w with w.stmt# = c.value</t>
+  </si>
+  <si>
+    <t>While Constant</t>
+  </si>
+  <si>
+    <t>if f;</t>
+  </si>
+  <si>
+    <t>Select f with f.stmt# = f.stmt#</t>
+  </si>
+  <si>
+    <t>If If</t>
+  </si>
+  <si>
+    <t>if f; prog_line pl;</t>
+  </si>
+  <si>
+    <t>Select f with f.stmt# = pl</t>
+  </si>
+  <si>
+    <t>If ProgLine</t>
+  </si>
+  <si>
+    <t>if f; call cl;</t>
+  </si>
+  <si>
+    <t>Select f with f.stmt# = cl.stmt#</t>
+  </si>
+  <si>
+    <t>If Call</t>
+  </si>
+  <si>
+    <t>if f; constant c;</t>
+  </si>
+  <si>
+    <t>Select f with f.stmt# = c.value</t>
+  </si>
+  <si>
+    <t>If Constant</t>
+  </si>
+  <si>
+    <t>Select pl with pl = pl;</t>
+  </si>
+  <si>
+    <t>ProgLine ProgLine</t>
+  </si>
+  <si>
+    <t>prog_line pl; call cl;</t>
+  </si>
+  <si>
+    <t>Select pl with pl = cl.stmt#</t>
+  </si>
+  <si>
+    <t>ProgLine Call</t>
+  </si>
+  <si>
+    <t>prog_line pl; constant cl</t>
+  </si>
+  <si>
+    <t>Select pl with pl = c.value</t>
+  </si>
+  <si>
+    <t>ProgLine Constant</t>
+  </si>
+  <si>
+    <t>Select cl with cl.stmt# = cl.stmt#</t>
+  </si>
+  <si>
+    <t>Call Call</t>
+  </si>
+  <si>
+    <t>Select cl with cl.stmt# = c.value</t>
+  </si>
+  <si>
+    <t>call cl; constant c;</t>
+  </si>
+  <si>
+    <t>Call Constant</t>
+  </si>
+  <si>
+    <t>Select c with c.value = c.value</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,8,9,10,20</t>
+  </si>
+  <si>
+    <t>Constant Constant</t>
+  </si>
+  <si>
+    <t>Select v with "a" = v.varName</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Ident Variable</t>
+  </si>
+  <si>
+    <t>Select v with "nonExist" = v.varName</t>
+  </si>
+  <si>
+    <t>Ident Procedure</t>
+  </si>
+  <si>
+    <t>Select p with "Sequential" = p.procName</t>
+  </si>
+  <si>
+    <t>Sequential</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN "Hi" = "Hi"</t>
+  </si>
+  <si>
+    <t>Ident Ident</t>
+  </si>
+  <si>
+    <t>Int Ident</t>
+  </si>
+  <si>
+    <t>Ident Int</t>
+  </si>
+  <si>
+    <t>Select cl with "TestJumpOverLoop" = cl.procName</t>
+  </si>
+  <si>
+    <t>Ident Call</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN v.varName = p.procName</t>
+  </si>
+  <si>
+    <t>Variable Procedure</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN v.varName = cl.procName</t>
+  </si>
+  <si>
+    <t>variable v; procedure p;</t>
+  </si>
+  <si>
+    <t>variable v; call cl;</t>
+  </si>
+  <si>
+    <t>Variable Call</t>
+  </si>
+  <si>
+    <t>procedure p; call cl;</t>
+  </si>
+  <si>
+    <t>Select BOOLEAN p.procName = c.procName</t>
+  </si>
+  <si>
+    <t>Procedure Call</t>
+  </si>
+  <si>
+    <t>stmt s; if f;</t>
+  </si>
+  <si>
+    <t>Select a with a.stmt# = c.value</t>
   </si>
 </sst>
 </file>
@@ -665,7 +1058,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF57BB8A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE67C73"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1044,18 +1461,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3B02F3-8668-4835-B18A-9EFEA275CE21}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="4" customWidth="1"/>
     <col min="3" max="3" width="42.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="40.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="87.5703125" style="4" customWidth="1"/>
@@ -1087,12 +1504,1043 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>34</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>35</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>38</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>39</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>40</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>41</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>42</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>43</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>44</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>45</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>46</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>47</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>48</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>49</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>50</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>51</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>52</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>53</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>54</v>
+      </c>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>55</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>56</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>57</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>58</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>59</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>60</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>61</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>301</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="7" priority="27" operator="equal">
+  <conditionalFormatting sqref="G1:G10 G12:G1048576">
+    <cfRule type="cellIs" dxfId="9" priority="29" operator="equal">
       <formula>"BUG"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="30" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+      <formula>"BUG"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>